<commit_message>
css modified, hoc auth logic modified
</commit_message>
<xml_diff>
--- a/react_studyl.xlsx
+++ b/react_studyl.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lyuls\Desktop\SpringStudy\myShoppingmall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D71F13A-BFA5-43C3-8B83-5FB81E285D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358DE48E-D921-418E-865F-29484C518617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="15600" xr2:uid="{DF666678-7982-4834-98A7-D57D5FE19ABE}"/>
   </bookViews>
   <sheets>
-    <sheet name="server" sheetId="1" r:id="rId1"/>
-    <sheet name="router 뼈대" sheetId="10" r:id="rId2"/>
-    <sheet name="db" sheetId="11" r:id="rId3"/>
-    <sheet name="node.js 통신방법" sheetId="2" r:id="rId4"/>
-    <sheet name="react 개념정리" sheetId="3" r:id="rId5"/>
-    <sheet name="client" sheetId="4" r:id="rId6"/>
-    <sheet name="login.js" sheetId="5" r:id="rId7"/>
-    <sheet name="landingPage.js" sheetId="9" r:id="rId8"/>
-    <sheet name="App.js" sheetId="8" r:id="rId9"/>
-    <sheet name="cookie" sheetId="7" r:id="rId10"/>
-    <sheet name="react hook정리" sheetId="6" r:id="rId11"/>
+    <sheet name="참고 링크" sheetId="12" r:id="rId1"/>
+    <sheet name="server" sheetId="1" r:id="rId2"/>
+    <sheet name="router 뼈대" sheetId="10" r:id="rId3"/>
+    <sheet name="db" sheetId="11" r:id="rId4"/>
+    <sheet name="node.js 통신방법" sheetId="2" r:id="rId5"/>
+    <sheet name="react 개념정리" sheetId="3" r:id="rId6"/>
+    <sheet name="client" sheetId="4" r:id="rId7"/>
+    <sheet name="login.js" sheetId="5" r:id="rId8"/>
+    <sheet name="landingPage.js" sheetId="9" r:id="rId9"/>
+    <sheet name="App.js" sheetId="8" r:id="rId10"/>
+    <sheet name="cookie" sheetId="7" r:id="rId11"/>
+    <sheet name="react hook정리" sheetId="6" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="278">
   <si>
     <t>3. node js의 프레임워크인 expess download</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1145,6 +1146,15 @@
   </si>
   <si>
     <t>app.use("/resources", express.static("resources"));</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/CSS/CSS_Flexible_Box_Layout/Basic_Concepts_of_Flexbox</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/CSS/float</t>
+  </si>
+  <si>
+    <t>https://flexboxfroggy.com/#ko</t>
   </si>
 </sst>
 </file>
@@ -1697,10 +1707,478 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B612749-3015-45EB-A02E-6B13AA008A73}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F655D294-A3F7-4F2F-9AC6-2E237EE25314}">
+  <dimension ref="A1:B62"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="B11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="B12" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="B13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="B14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="B15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="B16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" t="s">
+        <v>212</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA716FD-B4F5-426F-B791-AC02811AD324}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="B11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="B12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="B13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="B14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="B15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="B16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B550DD-E16D-4368-AD5F-A2C4609E2BD9}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>270</v>
+      </c>
+      <c r="B8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9" t="s">
+        <v>272</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0EF9A1C-62A0-4C1C-A226-5AC1B22DB405}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1818,138 +2296,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA716FD-B4F5-426F-B791-AC02811AD324}">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="B4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="B5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="B6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="B7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="B8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="B9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="B10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="B11" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="B12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="B13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="B14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="B15" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="B16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B550DD-E16D-4368-AD5F-A2C4609E2BD9}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>270</v>
-      </c>
-      <c r="B8" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="B9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19604161-C0DE-4EF1-8559-6904012A3B0B}">
   <dimension ref="A1:B49"/>
   <sheetViews>
@@ -2130,7 +2477,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20145887-F7CF-4D64-AC77-D45701735D7F}">
   <dimension ref="B3:B23"/>
   <sheetViews>
@@ -2241,7 +2588,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75B85B43-8BF0-40A2-B254-406BE1FF90AD}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -2312,7 +2659,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B72455-CA51-4F65-A021-773E9B30B4C5}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -2379,7 +2726,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4599B3D-2EBE-475E-BA0C-2DA09DF77F39}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -2647,7 +2994,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE339A7-BBA8-4CAC-9023-E22154281404}">
   <dimension ref="A1:B83"/>
   <sheetViews>
@@ -3053,7 +3400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E82F2D5-6CEB-4CFE-B37C-AED25CD7AE2C}">
   <dimension ref="B4:B26"/>
   <sheetViews>
@@ -3177,310 +3524,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F655D294-A3F7-4F2F-9AC6-2E237EE25314}">
-  <dimension ref="A1:B62"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="B4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="B5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="B6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="B7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="B8" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="B9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="B10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="B11" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="B12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="B13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="B14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="B15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="B16" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2">
-      <c r="B27" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2">
-      <c r="B29" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2">
-      <c r="B31" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2">
-      <c r="B32" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2">
-      <c r="B39" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2">
-      <c r="B41" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2">
-      <c r="B42" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2">
-      <c r="B43" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2">
-      <c r="B44" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2">
-      <c r="B45" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2">
-      <c r="B46" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2">
-      <c r="B47" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2">
-      <c r="B48" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2">
-      <c r="B50" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2">
-      <c r="B52" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2">
-      <c r="B53" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2">
-      <c r="B54" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2">
-      <c r="B55" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2">
-      <c r="B56" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2">
-      <c r="B57" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2">
-      <c r="B58" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2">
-      <c r="B59" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="60" spans="2:2">
-      <c r="B60" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2">
-      <c r="B62" t="s">
-        <v>212</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>